<commit_message>
Updated some SQL data to Excel Sheet code
</commit_message>
<xml_diff>
--- a/RegressionResults/YourNameHere/ExcelResults/RunResults.xlsx
+++ b/RegressionResults/YourNameHere/ExcelResults/RunResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sami/eclipse-workspace/JenkinsCucumber/RegressionResults/ssabir/ExcelResults/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sami/Desktop/GitTechTekSolution/SDETautomation/RegressionResults/YourNameHere/ExcelResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D44262-13EF-CA46-8B4D-A89CA73381D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7251466-F8CD-024A-B5AD-A7C8385F26D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,17 +398,17 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>